<commit_message>
Logins and dates updated
</commit_message>
<xml_diff>
--- a/docs/migration/dt/Mail2UPN_Migrationsuebersicht_UniBE.xlsx
+++ b/docs/migration/dt/Mail2UPN_Migrationsuebersicht_UniBE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibe365.sharepoint.com/sites/ID-Mail2UPN/Freigegebene Dokumente/Migrationen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{F666B896-236D-4007-90DF-EF40164E4F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D00CA408-4DE1-4519-B54B-A0E758375985}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{F666B896-236D-4007-90DF-EF40164E4F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D23C063C-2E5A-45F6-8696-9313D971A880}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{04BB4B5D-ED8C-450E-A019-A49FAF05B40D}"/>
+    <workbookView xWindow="3456" yWindow="2148" windowWidth="23040" windowHeight="14532" xr2:uid="{04BB4B5D-ED8C-450E-A019-A49FAF05B40D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Datum</t>
   </si>
@@ -300,6 +300,9 @@
       </rPr>
       <t xml:space="preserve"> Nachmigrationen</t>
     </r>
+  </si>
+  <si>
+    <t>CSH, SPACE</t>
   </si>
 </sst>
 </file>
@@ -790,6 +793,9 @@
       <c r="B11" s="4">
         <v>44356</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
@@ -1278,6 +1284,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101000B5FCF74A1A49E448305B6D279E916BF" ma:contentTypeVersion="8" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="4319ab122f5e0bfcf964c68c7fd55b84">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0859a3a8-2591-46fb-991a-bdfafc264af6" xmlns:ns3="817d9ee2-9f35-47f3-85a8-1c4f9e5679d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0951b72d2704573793f3023cca08553b" ns2:_="" ns3:_="">
     <xsd:import namespace="0859a3a8-2591-46fb-991a-bdfafc264af6"/>
@@ -1468,15 +1483,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1484,6 +1490,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D71FE82-3B51-4CD1-857A-863DD2419C08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16811ED4-1849-4AF4-9CBB-305406C7FCFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1498,14 +1512,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D71FE82-3B51-4CD1-857A-863DD2419C08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>